<commit_message>
Add Ash name to test file and add a question to QC excel file
</commit_message>
<xml_diff>
--- a/0921_Q&A Sheet.xlsx
+++ b/0921_Q&A Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kogam\GoogleDrive\CU_MSDS_CL\Capstone\JPMC3-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sience\GitHub\JPMC3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6CE1B3-7911-42B2-AE63-C2EAD451A178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2359BC65-9A48-4068-AB57-F3F49AC752C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -109,6 +107,12 @@
       </rPr>
       <t>'s Question</t>
     </r>
+  </si>
+  <si>
+    <t>IS there any Sample projects like this?</t>
+  </si>
+  <si>
+    <t>Ashkan</t>
   </si>
 </sst>
 </file>
@@ -462,8 +466,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -479,7 +483,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -781,19 +785,19 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" customWidth="1"/>
-    <col min="6" max="6" width="33.453125" customWidth="1"/>
-    <col min="8" max="8" width="29.7265625" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -843,19 +847,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10">
+        <v>44825</v>
+      </c>
       <c r="E3" s="14"/>
       <c r="F3" s="24"/>
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -867,7 +877,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -879,7 +889,7 @@
       <c r="G5" s="25"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -891,7 +901,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -903,7 +913,7 @@
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -915,7 +925,7 @@
       <c r="G8" s="25"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -927,7 +937,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -939,7 +949,7 @@
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -951,7 +961,7 @@
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -963,7 +973,7 @@
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -975,7 +985,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -987,7 +997,7 @@
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -999,7 +1009,7 @@
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1011,7 +1021,7 @@
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1023,7 +1033,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1035,7 +1045,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1047,7 +1057,7 @@
       <c r="G19" s="25"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1059,7 +1069,7 @@
       <c r="G20" s="25"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1071,7 +1081,7 @@
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
modified and added QAs
</commit_message>
<xml_diff>
--- a/0921_Q&A Sheet.xlsx
+++ b/0921_Q&A Sheet.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt2y1\OneDrive\デスクトップ\Columbia\Courses\Capstone\Landcover-Change-Detection-from-Satellite-Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA96B13-78A9-40E8-9188-C290FFEE9B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205381CC-A17D-4839-9273-CF888DC0CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="QA" sheetId="1" r:id="rId1"/>
+    <sheet name="supplementary note" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -121,12 +122,105 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t xml:space="preserve">We might use information such as the high possibility that X and Y are geographically adjacent to each other, and what the shape of X is most likely to be as inductive biases or Bayesian priors. The problem here is that such information varies by country and region. For example, Maryland has an image of having a lot of greenery, but it can be inferred that the ratio of urban areas is high in the vicinity of New York City. There will be heaven and earth differences between the Northeast and the Midwest of the United States. Not to mention the Amazon Basin and the Sahara Desert. So I would like to ask you, do you want this system to be made to fit a specific country or region (especially around New York City), or do you want it to be made to be universally applicable (instead, the accuracy in the neighborhood of New York City may be degraded)  </t>
+    <t>ID</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Masa
-Yuki</t>
+    <t>Supplementary note</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>back to QA</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Why do I ask this? See the note in supplementary note sheet</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Do you know git or python codes of 1st or 2nd winner teams of the MSD contest 2021? I could not find them.
+(You only share us the one for the base models)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Can we use not only NLCD but also Landsat for Meryland or possibly any other regions?</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Can we use some computational resource offered by JP Morgan (e.g. Google Cloud)?</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As Saba said in the first meeting, we want to detect the change </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in New York state</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (using models trained by available data, e.g. for Meryland), right?</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the answer for Q2 is YES, do we need to get the satellite images and make high-resolution labels of New York state for validation using GEE API etc </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>by ourselves</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?
+We may also want to have low-resolution labels of New York state for train.</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Do you want this system to be made to fit to a specific country or region (e.g. especially New York state) most, or do you want it to be made to be universally applicable to all over the world?</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Based on the answer for Q4, can we get additional data other than Meryland (e.g. other regions in US similar to New York state), if we want?</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>If we get images of New York state or some other regions, are we recommended to specify summer as the season?</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>We reasonably assume that JPMorgan wants to use the model not only New York state but also around the world. But, models might use information such as the high possibility that X and Y are geographically adjacent to each other or what the shape of X is most likely to be as inductive biases or Bayesian priors. The problem here is that such information varies by country and region. For example, Maryland has an image of having a lot of greenery, but it can be inferred that the ratio of urban areas is high in the vicinity of New York City. There will be heaven and earth differences between the Northeast and the Midwest of the United States. Not to mention the Amazon Basin and the Sahara Desert. So I would like to ask you, do you want this system to be made to fit a specific country or region (e.g. especially New York state), or do you want it to be made to be universally applicable (instead, the accuracy for New York state may be degraded).</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -134,7 +228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +259,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -431,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -489,6 +592,28 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -805,20 +930,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708A9855-82BB-4FE2-AC0B-07B016DC1B85}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.3984375" customWidth="1"/>
-    <col min="5" max="5" width="21.296875" customWidth="1"/>
+    <col min="5" max="5" width="22.796875" customWidth="1"/>
     <col min="6" max="6" width="33.3984375" customWidth="1"/>
     <col min="8" max="8" width="29.69921875" customWidth="1"/>
   </cols>
@@ -875,6 +1000,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
+        <f>ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -891,109 +1017,156 @@
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="342" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
+        <f t="shared" ref="A4:A31" si="0">ROW()-2</f>
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>14</v>
+      <c r="B4" s="32" t="s">
+        <v>22</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="30">
-        <v>44831</v>
+      <c r="D4" s="10">
+        <v>44836</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="24"/>
       <c r="G4" s="25"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="270" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="30">
-        <v>44831</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="10">
+        <v>44836</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="24"/>
       <c r="G5" s="25"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
+      <c r="B6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44836</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="24"/>
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="54" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+      <c r="B7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44836</v>
+      </c>
+      <c r="E7" s="36"/>
       <c r="F7" s="24"/>
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="54" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44836</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="F8" s="24"/>
       <c r="G8" s="25"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="54" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10">
+        <v>44836</v>
+      </c>
       <c r="E9" s="14"/>
       <c r="F9" s="24"/>
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="36" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="10">
+        <v>44836</v>
+      </c>
       <c r="E10" s="14"/>
       <c r="F10" s="24"/>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44836</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="24"/>
       <c r="G11" s="25"/>
@@ -1001,11 +1174,12 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="14"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
@@ -1013,11 +1187,12 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="14"/>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
@@ -1025,11 +1200,12 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="14"/>
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
@@ -1037,6 +1213,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="12"/>
@@ -1049,6 +1226,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="12"/>
@@ -1061,6 +1239,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="12"/>
@@ -1073,6 +1252,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B18" s="12"/>
@@ -1085,6 +1265,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19" s="12"/>
@@ -1097,6 +1278,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B20" s="12"/>
@@ -1109,6 +1291,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B21" s="12"/>
@@ -1119,24 +1302,243 @@
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="29"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="3">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{6489F446-2EDD-40F4-BDF1-09848BD43F07}"/>
+    <hyperlink ref="E8" location="'supplementary note'!B3" display="Why do I ask this? See note in supplementary note sheet" xr:uid="{250F3D91-A644-4255-88FB-F9D33F21AEF6}"/>
+    <hyperlink ref="E6" location="'supplementary note'!B2" display="Why do I ask this? See note in supplementary note sheet" xr:uid="{E784656E-2BF7-40A0-9ABF-55784DAB1583}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2345C9A5-90CC-49B0-B0EC-B7B801F0FC86}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="134.8984375" style="38" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" style="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="108" x14ac:dyDescent="0.45">
+      <c r="A2" s="34">
+        <v>4</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="126" x14ac:dyDescent="0.45">
+      <c r="A3" s="34">
+        <v>5</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="34"/>
+      <c r="B4" s="37"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="34"/>
+      <c r="B5" s="37"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="34"/>
+      <c r="B6" s="37"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="34"/>
+      <c r="B7" s="37"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="34"/>
+      <c r="B8" s="37"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="34"/>
+      <c r="B9" s="37"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="34"/>
+      <c r="B10" s="37"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="34"/>
+      <c r="B11" s="37"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="34"/>
+      <c r="B12" s="37"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="34"/>
+      <c r="B13" s="37"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="34"/>
+      <c r="B14" s="37"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <hyperlinks>
+    <hyperlink ref="C2" location="QA!B6" display="back to QA" xr:uid="{92F20005-CBE8-4A95-8DAB-A88C51C05484}"/>
+    <hyperlink ref="C3" location="QA!B8" display="back to QA" xr:uid="{52BC2303-71DA-4C76-B19A-1ACD5A4B8A2F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a question to Q&A file
</commit_message>
<xml_diff>
--- a/0921_Q&A Sheet.xlsx
+++ b/0921_Q&A Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt2y1\OneDrive\デスクトップ\Columbia\Courses\Capstone\Landcover-Change-Detection-from-Satellite-Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sience\GitHub\JPMC3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA96B13-78A9-40E8-9188-C290FFEE9B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D96FD40-BB37-4449-A270-BC1706CA0319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -66,7 +66,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -76,7 +76,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -89,7 +89,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -99,7 +99,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -129,16 +129,19 @@
 Yuki</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>Just for clarification: for the resolution of the training image we have: the original image is high resolution (1m) and the label is low resolution (30m). For the test, both images and labels are high resolutions (1m)? I ask because I am sure about the input training (not label) images resolution (I thought It was 30 same as its label but the paper says it is 1m)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -146,7 +149,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -154,13 +157,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -492,8 +495,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -509,7 +512,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -808,22 +811,22 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.3984375" customWidth="1"/>
-    <col min="5" max="5" width="21.296875" customWidth="1"/>
-    <col min="6" max="6" width="33.3984375" customWidth="1"/>
-    <col min="8" max="8" width="29.69921875" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,7 +852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -873,7 +876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -891,7 +894,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="342" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="300">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -909,7 +912,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="270" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="240">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -927,19 +930,25 @@
       <c r="G5" s="25"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="105">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="30">
+        <v>44836</v>
+      </c>
       <c r="E6" s="14"/>
       <c r="F6" s="24"/>
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -951,7 +960,7 @@
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -963,7 +972,7 @@
       <c r="G8" s="25"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -975,7 +984,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -987,7 +996,7 @@
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -999,7 +1008,7 @@
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1011,7 +1020,7 @@
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1023,7 +1032,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1035,7 +1044,7 @@
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1047,7 +1056,7 @@
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1059,7 +1068,7 @@
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1071,7 +1080,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1083,7 +1092,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1095,7 +1104,7 @@
       <c r="G19" s="25"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1107,7 +1116,7 @@
       <c r="G20" s="25"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1119,7 +1128,7 @@
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" s="4">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Resolve conflict and add Q to Q&A
</commit_message>
<xml_diff>
--- a/0921_Q&A Sheet.xlsx
+++ b/0921_Q&A Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt2y1\OneDrive\デスクトップ\Columbia\Courses\Capstone\Landcover-Change-Detection-from-Satellite-Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sience\GitHub\JPMC3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205381CC-A17D-4839-9273-CF888DC0CDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26669CD8-0F0E-4918-B952-42F59ED4FB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -67,7 +69,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -77,7 +79,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -90,7 +92,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -100,7 +102,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -159,7 +161,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -170,7 +172,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -187,7 +189,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -198,7 +200,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -223,16 +225,19 @@
     <t>We reasonably assume that JPMorgan wants to use the model not only New York state but also around the world. But, models might use information such as the high possibility that X and Y are geographically adjacent to each other or what the shape of X is most likely to be as inductive biases or Bayesian priors. The problem here is that such information varies by country and region. For example, Maryland has an image of having a lot of greenery, but it can be inferred that the ratio of urban areas is high in the vicinity of New York City. There will be heaven and earth differences between the Northeast and the Midwest of the United States. Not to mention the Amazon Basin and the Sahara Desert. So I would like to ask you, do you want this system to be made to fit a specific country or region (e.g. especially New York state), or do you want it to be made to be universally applicable (instead, the accuracy for New York state may be degraded).</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>Just for clarification: for the resolution of the training image we have: the original image is high resolution (1m) and the label is low resolution (30m). For the test, both images and labels are high resolutions (1m)? I ask because I am sure about the input training (not label) images resolution (I thought It was 30 same as its label but the paper says it is 1m)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -240,7 +245,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -248,13 +253,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -263,7 +268,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -617,8 +622,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -634,7 +639,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -933,22 +938,22 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.3984375" customWidth="1"/>
-    <col min="5" max="5" width="22.796875" customWidth="1"/>
-    <col min="6" max="6" width="33.3984375" customWidth="1"/>
-    <col min="8" max="8" width="29.69921875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -998,7 +1003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
         <f>ROW()-2</f>
         <v>1</v>
@@ -1017,7 +1022,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="45">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A31" si="0">ROW()-2</f>
         <v>2</v>
@@ -1036,7 +1041,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="90">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1055,7 +1060,7 @@
       <c r="G5" s="25"/>
       <c r="H5" s="26"/>
     </row>
-    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="60">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1076,7 +1081,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="45">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1094,7 +1099,7 @@
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="60">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1115,7 +1120,7 @@
       <c r="G8" s="25"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="45">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1134,7 +1139,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" ht="36" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1153,7 +1158,7 @@
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1172,20 +1177,26 @@
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="105">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="10"/>
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="10">
+        <v>44836</v>
+      </c>
       <c r="E12" s="14"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1198,7 +1209,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1211,7 +1222,7 @@
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1224,7 +1235,7 @@
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1237,7 +1248,7 @@
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1250,7 +1261,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1263,7 +1274,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1276,7 +1287,7 @@
       <c r="G19" s="25"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1289,7 +1300,7 @@
       <c r="G20" s="25"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1302,7 +1313,7 @@
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1315,7 +1326,7 @@
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1328,7 +1339,7 @@
       <c r="G23" s="25"/>
       <c r="H23" s="26"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1341,7 +1352,7 @@
       <c r="G24" s="25"/>
       <c r="H24" s="26"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1354,7 +1365,7 @@
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1367,7 +1378,7 @@
       <c r="G26" s="25"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1380,7 +1391,7 @@
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1393,7 +1404,7 @@
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1406,7 +1417,7 @@
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1419,7 +1430,7 @@
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1453,13 +1464,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="134.8984375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.85546875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="34" t="s">
         <v>15</v>
       </c>
@@ -1467,7 +1478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="108" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="105">
       <c r="A2" s="34">
         <v>4</v>
       </c>
@@ -1478,7 +1489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="126" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="120">
       <c r="A3" s="34">
         <v>5</v>
       </c>
@@ -1489,47 +1500,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4" s="34"/>
       <c r="B4" s="37"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5" s="34"/>
       <c r="B5" s="37"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6" s="34"/>
       <c r="B6" s="37"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7" s="34"/>
       <c r="B7" s="37"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8" s="34"/>
       <c r="B8" s="37"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9" s="34"/>
       <c r="B9" s="37"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10" s="34"/>
       <c r="B10" s="37"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11" s="34"/>
       <c r="B11" s="37"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12" s="34"/>
       <c r="B12" s="37"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13" s="34"/>
       <c r="B13" s="37"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14" s="34"/>
       <c r="B14" s="37"/>
     </row>

</xml_diff>

<commit_message>
Add 1 q to Q&A file
</commit_message>
<xml_diff>
--- a/0921_Q&A Sheet.xlsx
+++ b/0921_Q&A Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sience\GitHub\JPMC3-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26669CD8-0F0E-4918-B952-42F59ED4FB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5931780F-6F55-4B28-8120-648932100EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{62FED95C-DD31-4578-9215-DF44EF2F250C}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Just for clarification: for the resolution of the training image we have: the original image is high resolution (1m) and the label is low resolution (30m). For the test, both images and labels are high resolutions (1m)? I ask because I am sure about the input training (not label) images resolution (I thought It was 30 same as its label but the paper says it is 1m)</t>
+    <t>Just for clarification: for the resolution of the training image we have: the original image is high resolution (1m) and the label is low resolution (30m). For the test, both images and labels are high resolutions (1m)? I ask because I am sure about the input training (not label) images resolution (I thought It was 30 same as its label but the paper says it is 1m).</t>
   </si>
 </sst>
 </file>
@@ -938,10 +938,10 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>